<commit_message>
Update server.py and requirements.txt for robust Excel reading
</commit_message>
<xml_diff>
--- a/restaurants.xlsx
+++ b/restaurants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kroli\PycharmProjects\MAP_JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDD159-7C4D-436E-9BE5-EEFCAEF15369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF088F3-BB6B-4921-92C4-808B87926297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{38334122-D6CB-41C0-898C-DC56B1951378}"/>
   </bookViews>
@@ -1703,7 +1703,7 @@
   <dimension ref="A1:P128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,7 +5074,7 @@
         <v>30.431221000000001</v>
       </c>
       <c r="E119" s="6">
-        <v>45774</v>
+        <v>45773</v>
       </c>
       <c r="F119" t="s">
         <v>3</v>

</xml_diff>